<commit_message>
part of skill & code polish
</commit_message>
<xml_diff>
--- a/Data/ExtraEntryDesc.xlsx
+++ b/Data/ExtraEntryDesc.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -47,19 +47,37 @@
     <t>隐身</t>
   </si>
   <si>
-    <t>隐身状态下，敌方无法选中你作为目标，自身攻击后退出隐身状态</t>
+    <t>隐身状态下，敌方无法选中你作为目标，持续时间结束或自身攻击后退出隐身状态</t>
   </si>
   <si>
     <t>流血</t>
   </si>
   <si>
+    <t>拥有流血状态的角色受到伤害时，额外受到流血层数的伤害</t>
+  </si>
+  <si>
+    <t>击退</t>
+  </si>
+  <si>
+    <t>根据双方位置连成的直线，击退一格</t>
+  </si>
+  <si>
+    <t>念力</t>
+  </si>
+  <si>
+    <t>拥有念力的角色在造成伤害时，额外造成念力层数的伤害</t>
+  </si>
+  <si>
+    <t>腐蚀</t>
+  </si>
+  <si>
     <t>拥有流血状态的角色回合开始时受到一次流血层数的伤害</t>
   </si>
   <si>
-    <t>击退</t>
-  </si>
-  <si>
-    <t>根据双方位置连成的直线，击退一格</t>
+    <t>额外回合</t>
+  </si>
+  <si>
+    <t>不消耗buff持续时间的特殊回合</t>
   </si>
 </sst>
 </file>
@@ -1204,13 +1222,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="14.8942307692308" customWidth="1"/>
     <col min="3" max="3" width="191.5" customWidth="1"/>
@@ -1271,6 +1289,39 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>